<commit_message>
1. Update week 7
</commit_message>
<xml_diff>
--- a/10 Project Management/Project Plan/G33_QLNhaSach_WBS_RiskManagement.xlsx
+++ b/10 Project Management/Project Plan/G33_QLNhaSach_WBS_RiskManagement.xlsx
@@ -1414,7 +1414,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,7 +1693,9 @@
       <c r="E14" s="11">
         <v>43978</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="70">
+        <v>1</v>
+      </c>
       <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1710,7 +1712,9 @@
       <c r="E15" s="11">
         <v>43982</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="70">
+        <v>1</v>
+      </c>
       <c r="G15" s="28"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2936,6 +2940,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B4E384B51CAAB418E7EEC74982D28EA" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6f64d518e529f24b8b9618bd002d036">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0967b7be50301903c78f9c39c6fd9af8">
     <xsd:element name="properties">
@@ -3049,33 +3068,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56272AD9-7EF9-4089-861E-3BA6AD05A50B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDA7C492-E547-49B6-920E-3A57B3D94207}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3096,9 +3092,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDA7C492-E547-49B6-920E-3A57B3D94207}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56272AD9-7EF9-4089-861E-3BA6AD05A50B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1. Update week 8, 9
</commit_message>
<xml_diff>
--- a/10 Project Management/Project Plan/G33_QLNhaSach_WBS_RiskManagement.xlsx
+++ b/10 Project Management/Project Plan/G33_QLNhaSach_WBS_RiskManagement.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="142">
   <si>
     <t>Task</t>
   </si>
@@ -246,15 +246,6 @@
     <t>Cài đặt và đánh giá giao diện</t>
   </si>
   <si>
-    <t>Cài đặt module</t>
-  </si>
-  <si>
-    <t>kiểm thử module</t>
-  </si>
-  <si>
-    <t>Tích hợp hệ thống</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ghi nhận và sửa lỗi </t>
   </si>
   <si>
@@ -327,9 +318,6 @@
     <t>Laptop hoặc máy tính bị hỏng,…</t>
   </si>
   <si>
-    <t>Version: 3.6.2</t>
-  </si>
-  <si>
     <t>Version: 24.0.2</t>
   </si>
   <si>
@@ -469,6 +457,9 @@
   </si>
   <si>
     <t>SourceTree, Github</t>
+  </si>
+  <si>
+    <t>Version: 4.0</t>
   </si>
 </sst>
 </file>
@@ -972,9 +963,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -999,9 +987,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1054,6 +1039,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1414,7 +1405,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,25 +1418,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="61" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1456,7 +1447,7 @@
       <c r="B2" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="49" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="25">
@@ -1484,7 +1475,7 @@
       <c r="E3" s="11">
         <v>43940</v>
       </c>
-      <c r="F3" s="70">
+      <c r="F3" s="68">
         <v>1</v>
       </c>
       <c r="G3" s="28"/>
@@ -1503,7 +1494,7 @@
       <c r="E4" s="11">
         <v>43943</v>
       </c>
-      <c r="F4" s="70">
+      <c r="F4" s="68">
         <v>1</v>
       </c>
       <c r="G4" s="28"/>
@@ -1522,7 +1513,7 @@
       <c r="E5" s="11">
         <v>43947</v>
       </c>
-      <c r="F5" s="70">
+      <c r="F5" s="68">
         <v>1</v>
       </c>
       <c r="G5" s="28"/>
@@ -1541,7 +1532,7 @@
       <c r="E6" s="11">
         <v>43950</v>
       </c>
-      <c r="F6" s="70">
+      <c r="F6" s="68">
         <v>1</v>
       </c>
       <c r="G6" s="28"/>
@@ -1560,7 +1551,7 @@
       <c r="E7" s="11">
         <v>43954</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="68">
         <v>1</v>
       </c>
       <c r="G7" s="28"/>
@@ -1579,7 +1570,7 @@
       <c r="E8" s="11">
         <v>43957</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="68">
         <v>1</v>
       </c>
       <c r="G8" s="28"/>
@@ -1598,7 +1589,7 @@
       <c r="E9" s="11">
         <v>43961</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="68">
         <v>1</v>
       </c>
       <c r="G9" s="28"/>
@@ -1617,7 +1608,7 @@
       <c r="E10" s="11">
         <v>43964</v>
       </c>
-      <c r="F10" s="70">
+      <c r="F10" s="68">
         <v>1</v>
       </c>
       <c r="G10" s="28"/>
@@ -1636,7 +1627,7 @@
       <c r="E11" s="11">
         <v>43968</v>
       </c>
-      <c r="F11" s="70">
+      <c r="F11" s="68">
         <v>1</v>
       </c>
       <c r="G11" s="28"/>
@@ -1655,7 +1646,7 @@
       <c r="E12" s="11">
         <v>43971</v>
       </c>
-      <c r="F12" s="70">
+      <c r="F12" s="68">
         <v>1</v>
       </c>
       <c r="G12" s="28"/>
@@ -1674,7 +1665,7 @@
       <c r="E13" s="11">
         <v>43975</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="68">
         <v>1</v>
       </c>
       <c r="G13" s="28"/>
@@ -1693,7 +1684,7 @@
       <c r="E14" s="11">
         <v>43978</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="68">
         <v>1</v>
       </c>
       <c r="G14" s="28"/>
@@ -1712,7 +1703,7 @@
       <c r="E15" s="11">
         <v>43982</v>
       </c>
-      <c r="F15" s="70">
+      <c r="F15" s="68">
         <v>1</v>
       </c>
       <c r="G15" s="28"/>
@@ -1731,7 +1722,9 @@
       <c r="E16" s="11">
         <v>43985</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="68">
+        <v>1</v>
+      </c>
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,7 +1741,9 @@
       <c r="E17" s="11">
         <v>43989</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="68">
+        <v>1</v>
+      </c>
       <c r="G17" s="28"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1765,34 +1760,36 @@
       <c r="E18" s="11">
         <v>43992</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="68">
+        <v>1</v>
+      </c>
       <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="39">
         <v>43996</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="39">
         <v>43996</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="41"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="40"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="49" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="13">
@@ -1801,15 +1798,17 @@
       <c r="E20" s="13">
         <v>43940</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="55" t="s">
-        <v>97</v>
+      <c r="F20" s="14">
+        <v>1</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="42" t="s">
-        <v>88</v>
+      <c r="A21" s="50"/>
+      <c r="B21" s="41" t="s">
+        <v>85</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>40</v>
@@ -1820,17 +1819,19 @@
       <c r="E21" s="13">
         <v>43940</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="68">
+        <v>1</v>
+      </c>
       <c r="G21" s="28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53"/>
-      <c r="B22" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="56" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="54" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="13">
@@ -1839,36 +1840,40 @@
       <c r="E22" s="13">
         <v>43940</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="70">
+        <v>1</v>
+      </c>
       <c r="G22" s="32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="50" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="44" t="s">
-        <v>90</v>
+      <c r="B23" s="43" t="s">
+        <v>87</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="45">
+      <c r="D23" s="44">
         <v>43934</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="44">
         <v>43951</v>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="57" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F23" s="70">
+        <v>1</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
-      <c r="B24" s="42" t="s">
-        <v>91</v>
+      <c r="B24" s="41" t="s">
+        <v>88</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>40</v>
@@ -1879,36 +1884,40 @@
       <c r="E24" s="17">
         <v>43951</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="64" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F24" s="70">
+        <v>1</v>
+      </c>
+      <c r="G24" s="62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="27"/>
-      <c r="B25" s="42" t="s">
-        <v>92</v>
+      <c r="B25" s="41" t="s">
+        <v>89</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="45">
+      <c r="D25" s="44">
         <v>43934</v>
       </c>
-      <c r="E25" s="45">
+      <c r="E25" s="44">
         <v>43951</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="65" t="s">
-        <v>112</v>
+      <c r="F25" s="70">
+        <v>1</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="45"/>
       <c r="B26" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D26" s="17">
@@ -1917,17 +1926,19 @@
       <c r="E26" s="17">
         <v>43951</v>
       </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="66" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="F26" s="22">
+        <v>0.7</v>
+      </c>
+      <c r="G26" s="64" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="45"/>
       <c r="B27" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C27" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D27" s="17">
@@ -1936,17 +1947,19 @@
       <c r="E27" s="17">
         <v>43951</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="66" t="s">
-        <v>125</v>
+      <c r="F27" s="70">
+        <v>1</v>
+      </c>
+      <c r="G27" s="64" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="47"/>
+      <c r="A28" s="45"/>
       <c r="B28" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C28" s="48" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="17">
@@ -1955,19 +1968,21 @@
       <c r="E28" s="17">
         <v>43951</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="66" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="70">
+        <v>1</v>
+      </c>
+      <c r="G28" s="64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="51" t="s">
+      <c r="C29" s="49" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="25">
@@ -1976,15 +1991,17 @@
       <c r="E29" s="25">
         <v>43939</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="70">
+        <v>1</v>
+      </c>
       <c r="G29" s="26"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="27"/>
       <c r="B30" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="11">
@@ -1993,15 +2010,17 @@
       <c r="E30" s="11">
         <v>43946</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="70">
+        <v>1</v>
+      </c>
       <c r="G30" s="28"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="27"/>
       <c r="B31" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D31" s="11">
@@ -2010,15 +2029,17 @@
       <c r="E31" s="11">
         <v>43953</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="70">
+        <v>0.8</v>
+      </c>
       <c r="G31" s="28"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="27"/>
       <c r="B32" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D32" s="11">
@@ -2027,150 +2048,110 @@
       <c r="E32" s="11">
         <v>43960</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="70">
+        <v>1</v>
+      </c>
       <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="46" t="s">
         <v>40</v>
       </c>
       <c r="D33" s="11">
-        <v>43962</v>
+        <v>43983</v>
       </c>
       <c r="E33" s="11">
-        <v>43967</v>
-      </c>
-      <c r="F33" s="1"/>
+        <v>43988</v>
+      </c>
+      <c r="F33" s="19"/>
       <c r="G33" s="28"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="33" t="s">
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="29"/>
+      <c r="B34" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="11">
-        <v>43969</v>
-      </c>
-      <c r="E34" s="11">
-        <v>43974</v>
-      </c>
-      <c r="F34" s="1"/>
+      <c r="C34" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="31">
+        <v>43990</v>
+      </c>
+      <c r="E34" s="31">
+        <v>43995</v>
+      </c>
+      <c r="F34" s="30"/>
       <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="33" t="s">
+      <c r="A35" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="11">
-        <v>43976</v>
-      </c>
-      <c r="E35" s="11">
-        <v>43981</v>
-      </c>
-      <c r="F35" s="1"/>
+      <c r="C35" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="25">
+        <v>43997</v>
+      </c>
+      <c r="E35" s="25">
+        <v>44002</v>
+      </c>
+      <c r="F35" s="24"/>
       <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>40</v>
+      <c r="C36" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="D36" s="11">
-        <v>43983</v>
+        <v>43997</v>
       </c>
       <c r="E36" s="11">
-        <v>43988</v>
-      </c>
-      <c r="F36" s="19"/>
-      <c r="G36" s="35"/>
+        <v>44002</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="34"/>
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29"/>
-      <c r="B37" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="60" t="s">
-        <v>42</v>
+      <c r="B37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="54" t="s">
+        <v>41</v>
       </c>
       <c r="D37" s="31">
-        <v>43990</v>
+        <v>43997</v>
       </c>
       <c r="E37" s="31">
-        <v>43995</v>
+        <v>44002</v>
       </c>
       <c r="F37" s="30"/>
       <c r="G37" s="32"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="25">
-        <v>43997</v>
-      </c>
-      <c r="E38" s="25">
-        <v>44002</v>
-      </c>
-      <c r="F38" s="24"/>
       <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="11">
-        <v>43997</v>
-      </c>
-      <c r="E39" s="11">
-        <v>44002</v>
-      </c>
-      <c r="F39" s="1"/>
       <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="29"/>
-      <c r="B40" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C40" s="56" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="31">
-        <v>43997</v>
-      </c>
-      <c r="E40" s="31">
-        <v>44002</v>
-      </c>
-      <c r="F40" s="30"/>
       <c r="G40" s="32"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20 A23 A29:A40 A26:A28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A20 A23 A26:A37">
       <formula1>Task_Group</formula1>
     </dataValidation>
   </dataValidations>
@@ -2183,7 +2164,7 @@
           <x14:formula1>
             <xm:f>Ref!$G$2:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C5 C29:C40 C7:C28</xm:sqref>
+          <xm:sqref>C2:C5 C7:C37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -2256,10 +2237,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>32</v>
@@ -2280,8 +2261,8 @@
       <c r="I2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="58" t="s">
-        <v>99</v>
+      <c r="J2" s="56" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2289,10 +2270,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>32</v>
@@ -2314,7 +2295,7 @@
         <v>36</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2322,10 +2303,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>32</v>
@@ -2347,7 +2328,7 @@
         <v>36</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2355,10 +2336,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>31</v>
@@ -2380,7 +2361,7 @@
         <v>36</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -2388,10 +2369,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>32</v>
@@ -2413,18 +2394,18 @@
         <v>36</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
+      <c r="A7" s="36">
         <v>6</v>
       </c>
-      <c r="B7" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>104</v>
+      <c r="B7" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>100</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>32</v>
@@ -2446,18 +2427,18 @@
         <v>37</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="43" t="s">
-        <v>93</v>
+      <c r="B8" s="42" t="s">
+        <v>90</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>31</v>
@@ -2479,7 +2460,7 @@
         <v>37</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
@@ -2487,10 +2468,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>29</v>
@@ -2512,7 +2493,7 @@
         <v>37</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2520,10 +2501,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>32</v>
@@ -2545,7 +2526,7 @@
         <v>38</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2554,10 +2535,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>31</v>
@@ -2579,7 +2560,7 @@
         <v>38</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2588,10 +2569,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>31</v>
@@ -2613,7 +2594,7 @@
         <v>37</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -2621,11 +2602,11 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B13" s="67" t="s">
-        <v>127</v>
+      <c r="B13" s="65" t="s">
+        <v>123</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>29</v>
@@ -2647,7 +2628,7 @@
         <v>37</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -2656,10 +2637,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="58" t="s">
-        <v>131</v>
+        <v>124</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>127</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>34</v>
@@ -2681,7 +2662,7 @@
         <v>38</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="63" x14ac:dyDescent="0.25">
@@ -2690,10 +2671,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>28</v>
@@ -2715,7 +2696,7 @@
         <v>36</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2902,35 +2883,35 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="69" t="s">
-        <v>137</v>
+      <c r="A10" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="67" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>